<commit_message>
run Merge branch 'main' of https://github.com/gellavenugopal/audit-assistant-pro-electron
</commit_message>
<xml_diff>
--- a/SRM_Pro/Mapping (1).xlsx
+++ b/SRM_Pro/Mapping (1).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ICAI_Audit_Tool\nw\SRM_Pro\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CED6E937-C6A3-4380-9319-51689DC677A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DA15B43-BC03-43DC-B417-2C6EF8BE6514}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{ADE66A2A-F2AB-4415-AE10-07E079855D41}"/>
   </bookViews>
@@ -439,7 +439,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -658,18 +658,16 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:AA813"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="A45" sqref="A45"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="223.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="122.5546875" customWidth="1"/>
     <col min="3" max="3" width="52.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="49" bestFit="1" customWidth="1"/>
-    <col min="5" max="8" width="24.6640625" customWidth="1"/>
-    <col min="9" max="9" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="7" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="77.21875" bestFit="1" customWidth="1"/>
     <col min="10" max="27" width="24.6640625" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>